<commit_message>
Adding data files for 10 companies
</commit_message>
<xml_diff>
--- a/data/Reliance.xlsx
+++ b/data/Reliance.xlsx
@@ -383,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7105"/>
+  <dimension ref="A1:B7119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -57229,6 +57229,118 @@
         <v>1926</v>
       </c>
     </row>
+    <row r="7106" spans="1:2">
+      <c r="A7106" s="2">
+        <v>44323</v>
+      </c>
+      <c r="B7106">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="7107" spans="1:2">
+      <c r="A7107" s="2">
+        <v>44326</v>
+      </c>
+      <c r="B7107">
+        <v>1943.75</v>
+      </c>
+    </row>
+    <row r="7108" spans="1:2">
+      <c r="A7108" s="2">
+        <v>44327</v>
+      </c>
+      <c r="B7108">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="7109" spans="1:2">
+      <c r="A7109" s="2">
+        <v>44328</v>
+      </c>
+      <c r="B7109">
+        <v>1934</v>
+      </c>
+    </row>
+    <row r="7110" spans="1:2">
+      <c r="A7110" s="2">
+        <v>44330</v>
+      </c>
+      <c r="B7110">
+        <v>1925.1</v>
+      </c>
+    </row>
+    <row r="7111" spans="1:2">
+      <c r="A7111" s="2">
+        <v>44333</v>
+      </c>
+      <c r="B7111">
+        <v>1938.7</v>
+      </c>
+    </row>
+    <row r="7112" spans="1:2">
+      <c r="A7112" s="2">
+        <v>44334</v>
+      </c>
+      <c r="B7112">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="7113" spans="1:2">
+      <c r="A7113" s="2">
+        <v>44335</v>
+      </c>
+      <c r="B7113">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="7114" spans="1:2">
+      <c r="A7114" s="2">
+        <v>44336</v>
+      </c>
+      <c r="B7114">
+        <v>1996.35</v>
+      </c>
+    </row>
+    <row r="7115" spans="1:2">
+      <c r="A7115" s="2">
+        <v>44337</v>
+      </c>
+      <c r="B7115">
+        <v>1995.7</v>
+      </c>
+    </row>
+    <row r="7116" spans="1:2">
+      <c r="A7116" s="2">
+        <v>44340</v>
+      </c>
+      <c r="B7116">
+        <v>2007.4</v>
+      </c>
+    </row>
+    <row r="7117" spans="1:2">
+      <c r="A7117" s="2">
+        <v>44341</v>
+      </c>
+      <c r="B7117">
+        <v>1990.05</v>
+      </c>
+    </row>
+    <row r="7118" spans="1:2">
+      <c r="A7118" s="2">
+        <v>44342</v>
+      </c>
+      <c r="B7118">
+        <v>1984.9</v>
+      </c>
+    </row>
+    <row r="7119" spans="1:2">
+      <c r="A7119" s="2">
+        <v>44343</v>
+      </c>
+      <c r="B7119">
+        <v>1970.9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>